<commit_message>
BITF, COIN Q3 UPDATE
</commit_message>
<xml_diff>
--- a/Retail Wholesale - Restaurants/CMG.xlsx
+++ b/Retail Wholesale - Restaurants/CMG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\models\Retail Wholesale - Restaurants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009F708D-E74B-4A8B-9816-BE0991824078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC0B4DC-FE69-40B8-99CC-024E61F86611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -318,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="220">
   <si>
     <t>Price</t>
   </si>
@@ -975,6 +975,9 @@
   </si>
   <si>
     <t>Sales per Restaurant</t>
+  </si>
+  <si>
+    <t>Shares (diluted)</t>
   </si>
 </sst>
 </file>
@@ -1717,7 +1720,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1872,6 +1875,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1929,20 +1933,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -18987,7 +18977,7 @@
   <dimension ref="B2:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19118,7 +19108,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="13">
-        <v>58.3</v>
+        <v>58.8</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>161</v>
@@ -19144,8 +19134,8 @@
         <v>1</v>
       </c>
       <c r="C7" s="15">
-        <f>Model!Y21</f>
-        <v>1381.518</v>
+        <f>Model!Z21</f>
+        <v>1374.605</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>163</v>
@@ -19174,7 +19164,7 @@
       </c>
       <c r="C8" s="15">
         <f>C6*C7</f>
-        <v>80542.499400000001</v>
+        <v>80826.77399999999</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>165</v>
@@ -19202,8 +19192,8 @@
         <v>3</v>
       </c>
       <c r="C9" s="15">
-        <f>Model!Y37+Model!Y42</f>
-        <v>1489.8150000000001</v>
+        <f>Model!Z37+Model!Z42</f>
+        <v>1367.223</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>167</v>
@@ -19261,7 +19251,7 @@
       </c>
       <c r="C11" s="15">
         <f>C9-C10</f>
-        <v>1489.8150000000001</v>
+        <v>1367.223</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>171</v>
@@ -19290,7 +19280,7 @@
       </c>
       <c r="C12" s="15">
         <f>C8-C9+C10</f>
-        <v>79052.684399999998</v>
+        <v>79459.550999999992</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>173</v>
@@ -19319,7 +19309,7 @@
       </c>
       <c r="C13" s="36">
         <f>C6/Model!G22</f>
-        <v>64.777777777777771</v>
+        <v>65.333333333333329</v>
       </c>
       <c r="E13" s="5"/>
       <c r="J13" s="13"/>
@@ -19332,7 +19322,7 @@
       </c>
       <c r="C14" s="36">
         <f>C6/Model!H23</f>
-        <v>52.522522522522515</v>
+        <v>52.972972972972968</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="29"/>
@@ -19350,7 +19340,7 @@
       </c>
       <c r="C15" s="36">
         <f>C6/Model!I23</f>
-        <v>44.503816793893122</v>
+        <v>44.885496183206101</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
@@ -19373,9 +19363,9 @@
       <c r="E17" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="L17" s="124"/>
-      <c r="M17" s="125"/>
-      <c r="N17" s="126"/>
+      <c r="L17" s="125"/>
+      <c r="M17" s="126"/>
+      <c r="N17" s="127"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
@@ -19383,14 +19373,14 @@
       </c>
       <c r="C18" s="49">
         <f>C14/(C16*100)</f>
-        <v>2.2509652509652502</v>
+        <v>2.2702702702702693</v>
       </c>
       <c r="E18" t="s">
         <v>216</v>
       </c>
-      <c r="L18" s="127"/>
-      <c r="M18" s="128"/>
-      <c r="N18" s="129"/>
+      <c r="L18" s="128"/>
+      <c r="M18" s="129"/>
+      <c r="N18" s="130"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
@@ -19398,14 +19388,14 @@
       </c>
       <c r="C19" s="49">
         <f>C15/(C17*100)</f>
-        <v>2.469961832061069</v>
+        <v>2.4911450381679394</v>
       </c>
       <c r="E19" t="s">
         <v>217</v>
       </c>
-      <c r="L19" s="127"/>
-      <c r="M19" s="128"/>
-      <c r="N19" s="129"/>
+      <c r="L19" s="128"/>
+      <c r="M19" s="129"/>
+      <c r="N19" s="130"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -19418,9 +19408,9 @@
       <c r="E20" t="s">
         <v>218</v>
       </c>
-      <c r="L20" s="127"/>
-      <c r="M20" s="128"/>
-      <c r="N20" s="129"/>
+      <c r="L20" s="128"/>
+      <c r="M20" s="129"/>
+      <c r="N20" s="130"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
@@ -19430,9 +19420,9 @@
         <f>Model!I6/Model!H6-1</f>
         <v>0.13580246913580241</v>
       </c>
-      <c r="L21" s="127"/>
-      <c r="M21" s="128"/>
-      <c r="N21" s="129"/>
+      <c r="L21" s="128"/>
+      <c r="M21" s="129"/>
+      <c r="N21" s="130"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
@@ -19442,9 +19432,9 @@
         <f>Model!G16+Model!G13</f>
         <v>1877.2069999999983</v>
       </c>
-      <c r="L22" s="127"/>
-      <c r="M22" s="128"/>
-      <c r="N22" s="129"/>
+      <c r="L22" s="128"/>
+      <c r="M22" s="129"/>
+      <c r="N22" s="130"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
@@ -19454,33 +19444,33 @@
         <f>Model!G18</f>
         <v>1620.5059999999983</v>
       </c>
-      <c r="L23" s="127"/>
-      <c r="M23" s="128"/>
-      <c r="N23" s="129"/>
+      <c r="L23" s="128"/>
+      <c r="M23" s="129"/>
+      <c r="N23" s="130"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="7">
-        <f>Model!Y24</f>
-        <v>0.2890569055977279</v>
-      </c>
-      <c r="L24" s="127"/>
-      <c r="M24" s="128"/>
-      <c r="N24" s="129"/>
+        <f>Model!Z24</f>
+        <v>0.25493525144832285</v>
+      </c>
+      <c r="L24" s="128"/>
+      <c r="M24" s="129"/>
+      <c r="N24" s="130"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="7">
-        <f>Model!Y25</f>
-        <v>0.15326372961440815</v>
-      </c>
-      <c r="L25" s="127"/>
-      <c r="M25" s="128"/>
-      <c r="N25" s="129"/>
+        <f>Model!Z25</f>
+        <v>0.13867100805562471</v>
+      </c>
+      <c r="L25" s="128"/>
+      <c r="M25" s="129"/>
+      <c r="N25" s="130"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
@@ -19488,11 +19478,11 @@
       </c>
       <c r="C26" s="36">
         <f>C12/C23</f>
-        <v>48.782716262698244</v>
-      </c>
-      <c r="L26" s="127"/>
-      <c r="M26" s="128"/>
-      <c r="N26" s="129"/>
+        <v>49.033790063103794</v>
+      </c>
+      <c r="L26" s="128"/>
+      <c r="M26" s="129"/>
+      <c r="N26" s="130"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
@@ -19504,9 +19494,9 @@
       <c r="E27" t="s">
         <v>76</v>
       </c>
-      <c r="L27" s="127"/>
-      <c r="M27" s="128"/>
-      <c r="N27" s="129"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="129"/>
+      <c r="N27" s="130"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
@@ -19518,17 +19508,17 @@
       <c r="E28" t="s">
         <v>214</v>
       </c>
-      <c r="L28" s="130"/>
-      <c r="M28" s="131"/>
-      <c r="N28" s="132"/>
+      <c r="L28" s="131"/>
+      <c r="M28" s="132"/>
+      <c r="N28" s="133"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>84</v>
       </c>
       <c r="C29" s="36">
-        <f>Model!Y43/Model!Y57</f>
-        <v>1.7123977621755522</v>
+        <f>Model!Z43/Model!Z57</f>
+        <v>1.6189246582469716</v>
       </c>
       <c r="E29" t="s">
         <v>215</v>
@@ -19539,8 +19529,8 @@
         <v>85</v>
       </c>
       <c r="C30" s="36">
-        <f>(Model!Y37+Model!Y42)/Model!Y57</f>
-        <v>1.4281804447273467</v>
+        <f>(Model!Z37+Model!Z42)/Model!Z57</f>
+        <v>1.317317734929915</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
@@ -19548,8 +19538,8 @@
         <v>86</v>
       </c>
       <c r="C31" s="6">
-        <f>(Model!Y43-Model!Y57)/Model!Y50</f>
-        <v>8.331342451962398E-2</v>
+        <f>(Model!Z43-Model!Z57)/Model!Z50</f>
+        <v>7.1282237365549325E-2</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
@@ -19557,8 +19547,8 @@
         <v>87</v>
       </c>
       <c r="C32" s="36">
-        <f>(Model!Y50-Model!Y61)/C7</f>
-        <v>2.6867691915704324</v>
+        <f>(Model!Z50-Model!Z61)/C7</f>
+        <v>2.6290447073886676</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -19608,10 +19598,10 @@
   <dimension ref="A1:AB83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="V24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z16" sqref="Z16"/>
+      <selection pane="bottomRight" activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19619,7 +19609,6 @@
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="13"/>
-    <col min="25" max="25" width="11.42578125" style="143"/>
     <col min="26" max="26" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
@@ -19689,7 +19678,7 @@
       <c r="X2" t="s">
         <v>67</v>
       </c>
-      <c r="Y2" s="143" t="s">
+      <c r="Y2" t="s">
         <v>70</v>
       </c>
       <c r="Z2" s="13" t="s">
@@ -19760,7 +19749,7 @@
       <c r="X3" s="10">
         <v>2684.4470000000001</v>
       </c>
-      <c r="Y3" s="144">
+      <c r="Y3" s="10">
         <v>2954.913</v>
       </c>
       <c r="Z3" s="15">
@@ -19829,7 +19818,7 @@
       <c r="X4" s="10">
         <v>17.401</v>
       </c>
-      <c r="Y4" s="144">
+      <c r="Y4" s="10">
         <v>18.204000000000001</v>
       </c>
       <c r="Z4" s="15">
@@ -19919,7 +19908,7 @@
         <f t="shared" si="0"/>
         <v>2701.848</v>
       </c>
-      <c r="Y5" s="145">
+      <c r="Y5" s="11">
         <f t="shared" ref="Y5:AB5" si="1">SUM(Y3:Y4)</f>
         <v>2973.1170000000002</v>
       </c>
@@ -19980,14 +19969,14 @@
       <c r="X6" s="10">
         <v>2680</v>
       </c>
-      <c r="Y6" s="144"/>
-      <c r="Z6" s="152">
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="124">
         <v>2810</v>
       </c>
       <c r="AA6" s="10">
         <v>2850</v>
       </c>
-      <c r="AB6" s="151">
+      <c r="AB6" s="10">
         <v>3060</v>
       </c>
     </row>
@@ -20054,7 +20043,7 @@
       <c r="X7" s="10">
         <v>779.07600000000002</v>
       </c>
-      <c r="Y7" s="144">
+      <c r="Y7" s="10">
         <v>873.673</v>
       </c>
       <c r="Z7" s="15">
@@ -20125,7 +20114,7 @@
       <c r="X8" s="10">
         <v>659.45</v>
       </c>
-      <c r="Y8" s="144">
+      <c r="Y8" s="10">
         <v>716.62699999999995</v>
       </c>
       <c r="Z8" s="15">
@@ -20196,7 +20185,7 @@
       <c r="X9" s="10">
         <v>135.69900000000001</v>
       </c>
-      <c r="Y9" s="144">
+      <c r="Y9" s="10">
         <v>138.66300000000001</v>
       </c>
       <c r="Z9" s="15">
@@ -20267,7 +20256,7 @@
       <c r="X10" s="10">
         <v>385.77300000000002</v>
       </c>
-      <c r="Y10" s="144">
+      <c r="Y10" s="10">
         <v>384.75400000000002</v>
       </c>
       <c r="Z10" s="15">
@@ -20359,12 +20348,12 @@
         <f t="shared" ref="X11:AA11" si="18">SUM(X7:X10)</f>
         <v>1959.998</v>
       </c>
-      <c r="Y11" s="145">
+      <c r="Y11" s="11">
         <f t="shared" si="18"/>
         <v>2113.7170000000001</v>
       </c>
       <c r="Z11" s="14">
-        <f t="shared" si="18"/>
+        <f>SUM(Z7:Z10)</f>
         <v>2081.395</v>
       </c>
       <c r="AA11" s="11">
@@ -20441,7 +20430,7 @@
       <c r="X12" s="10">
         <v>204.625</v>
       </c>
-      <c r="Y12" s="144">
+      <c r="Y12" s="10">
         <v>175.02799999999999</v>
       </c>
       <c r="Z12" s="15">
@@ -20518,7 +20507,7 @@
       <c r="X13" s="10">
         <v>83.242999999999995</v>
       </c>
-      <c r="Y13" s="144">
+      <c r="Y13" s="10">
         <v>83.561999999999998</v>
       </c>
       <c r="Z13" s="15">
@@ -20595,7 +20584,7 @@
       <c r="X14" s="10">
         <v>7.2110000000000003</v>
       </c>
-      <c r="Y14" s="144">
+      <c r="Y14" s="10">
         <v>8.9949999999999992</v>
       </c>
       <c r="Z14" s="15">
@@ -20670,7 +20659,7 @@
       <c r="X15" s="10">
         <v>5.4790000000000001</v>
       </c>
-      <c r="Y15" s="144">
+      <c r="Y15" s="10">
         <v>5.7619999999999996</v>
       </c>
       <c r="Z15" s="15">
@@ -20764,7 +20753,7 @@
         <f t="shared" ref="X16:AA16" si="36">X5-SUM(X11:X15)</f>
         <v>441.29200000000037</v>
       </c>
-      <c r="Y16" s="145">
+      <c r="Y16" s="11">
         <f t="shared" si="36"/>
         <v>586.05300000000034</v>
       </c>
@@ -20844,10 +20833,12 @@
       <c r="X17" s="10">
         <v>19.364000000000001</v>
       </c>
-      <c r="Y17" s="144">
+      <c r="Y17" s="10">
         <v>21.861000000000001</v>
       </c>
-      <c r="Z17" s="15"/>
+      <c r="Z17" s="15">
+        <v>29.306999999999999</v>
+      </c>
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -20934,13 +20925,13 @@
         <f t="shared" si="38"/>
         <v>460.65600000000035</v>
       </c>
-      <c r="Y18" s="145">
+      <c r="Y18" s="11">
         <f t="shared" ref="Y18:AA18" si="39">Y16+SUM(Y17:Y17)</f>
         <v>607.91400000000033</v>
       </c>
       <c r="Z18" s="14">
         <f t="shared" si="39"/>
-        <v>473.25599999999986</v>
+        <v>502.56299999999987</v>
       </c>
       <c r="AA18" s="11">
         <f t="shared" si="39"/>
@@ -21016,10 +21007,12 @@
       <c r="X19" s="10">
         <v>101.369</v>
       </c>
-      <c r="Y19" s="144">
+      <c r="Y19" s="10">
         <v>152.24299999999999</v>
       </c>
-      <c r="Z19" s="15"/>
+      <c r="Z19" s="15">
+        <v>115.175</v>
+      </c>
       <c r="AA19" s="10"/>
     </row>
     <row r="20" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -21106,13 +21099,13 @@
         <f t="shared" si="40"/>
         <v>359.28700000000038</v>
       </c>
-      <c r="Y20" s="145">
+      <c r="Y20" s="11">
         <f t="shared" ref="Y20:AA20" si="41">Y18-SUM(Y19:Y19)</f>
         <v>455.67100000000033</v>
       </c>
       <c r="Z20" s="14">
         <f t="shared" si="41"/>
-        <v>473.25599999999986</v>
+        <v>387.38799999999986</v>
       </c>
       <c r="AA20" s="11">
         <f t="shared" si="41"/>
@@ -21121,7 +21114,7 @@
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>1</v>
+        <v>219</v>
       </c>
       <c r="C21" s="10">
         <v>28.295000000000002</v>
@@ -21183,10 +21176,12 @@
       <c r="X21" s="10">
         <v>27.623999999999999</v>
       </c>
-      <c r="Y21" s="144">
+      <c r="Y21" s="10">
         <v>1381.518</v>
       </c>
-      <c r="Z21" s="15"/>
+      <c r="Z21" s="15">
+        <v>1374.605</v>
+      </c>
       <c r="AA21" s="10"/>
     </row>
     <row r="22" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -21272,13 +21267,13 @@
         <f>X20/X21</f>
         <v>13.006335070952808</v>
       </c>
-      <c r="Y22" s="146">
+      <c r="Y22" s="47">
         <f t="shared" ref="Y22:AA22" si="43">Y20/Y21</f>
         <v>0.32983355989570917</v>
       </c>
-      <c r="Z22" s="46" t="e">
+      <c r="Z22" s="46">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>0.28181768580792288</v>
       </c>
       <c r="AA22" s="47" t="e">
         <f t="shared" si="43"/>
@@ -21329,9 +21324,9 @@
       <c r="X23" s="119">
         <v>11.69</v>
       </c>
-      <c r="Y23" s="147"/>
+      <c r="Y23" s="119"/>
       <c r="Z23" s="120"/>
-      <c r="AA23" s="119">
+      <c r="AA23" s="47">
         <v>0.24</v>
       </c>
       <c r="AB23" s="1">
@@ -21517,13 +21512,13 @@
         <f t="shared" ref="X25" si="48">X20/X5</f>
         <v>0.13297824303957897</v>
       </c>
-      <c r="Y25" s="148">
+      <c r="Y25" s="4">
         <f t="shared" ref="Y25:AA25" si="49">Y20/Y5</f>
         <v>0.15326372961440815</v>
       </c>
       <c r="Z25" s="7">
         <f t="shared" si="49"/>
-        <v>0.16940867189580661</v>
+        <v>0.13867100805562471</v>
       </c>
       <c r="AA25" s="4" t="e">
         <f t="shared" si="49"/>
@@ -21608,13 +21603,13 @@
         <f t="shared" si="51"/>
         <v>0.22005357577020579</v>
       </c>
-      <c r="Y26" s="148">
+      <c r="Y26" s="4">
         <f t="shared" si="51"/>
         <v>0.2504350944376999</v>
       </c>
       <c r="Z26" s="7">
         <f t="shared" ref="Z26:AA26" si="52">-Z19/Z18</f>
-        <v>0</v>
+        <v>-0.22917524768039038</v>
       </c>
       <c r="AA26" s="4" t="e">
         <f t="shared" si="52"/>
@@ -21690,7 +21685,7 @@
         <f t="shared" ref="X27" si="54">X5/T5-1</f>
         <v>0.14070371277305393</v>
       </c>
-      <c r="Y27" s="148">
+      <c r="Y27" s="4">
         <f t="shared" ref="Y27" si="55">Y5/U5-1</f>
         <v>0.18224742236065605</v>
       </c>
@@ -21785,7 +21780,7 @@
         <f t="shared" ref="X28" si="59">X12/X5</f>
         <v>7.573520049980606E-2</v>
       </c>
-      <c r="Y28" s="148">
+      <c r="Y28" s="4">
         <f t="shared" ref="Y28:AA28" si="60">Y12/Y5</f>
         <v>5.8870202551732739E-2</v>
       </c>
@@ -21880,7 +21875,7 @@
         <f t="shared" ref="X29" si="62">X13/X5</f>
         <v>3.0809653244742115E-2</v>
       </c>
-      <c r="Y29" s="148">
+      <c r="Y29" s="4">
         <f t="shared" ref="Y29:AA29" si="63">Y13/Y5</f>
         <v>2.810585658082073E-2</v>
       </c>
@@ -21975,7 +21970,7 @@
         <f t="shared" ref="X30" si="65">X15/X5</f>
         <v>2.0278712940180205E-3</v>
       </c>
-      <c r="Y30" s="148">
+      <c r="Y30" s="4">
         <f t="shared" ref="Y30:AA30" si="66">Y15/Y5</f>
         <v>1.938033383819069E-3</v>
       </c>
@@ -22051,7 +22046,7 @@
         <f>X3/T3-1</f>
         <v>0.14182761529198751</v>
       </c>
-      <c r="Y31" s="148">
+      <c r="Y31" s="4">
         <f t="shared" ref="Y31:AA31" si="69">Y3/U3-1</f>
         <v>0.18314408476606081</v>
       </c>
@@ -22127,7 +22122,7 @@
         <f>X4/T4-1</f>
         <v>-9.6750327243755319E-3</v>
       </c>
-      <c r="Y32" s="148">
+      <c r="Y32" s="4">
         <f t="shared" ref="Y32:AA32" si="71">Y4/U4-1</f>
         <v>5.2741151977793166E-2</v>
       </c>
@@ -22209,13 +22204,13 @@
         <f t="shared" ref="X33" si="73">X20/T20-1</f>
         <v>0.23193688195197204</v>
       </c>
-      <c r="Y33" s="148">
+      <c r="Y33" s="4">
         <f t="shared" ref="Y33" si="74">Y20/U20-1</f>
         <v>0.33287799455933498</v>
       </c>
       <c r="Z33" s="7">
         <f t="shared" ref="Z33" si="75">Z20/V20-1</f>
-        <v>0.51095247065133576</v>
+        <v>0.23680387718418716</v>
       </c>
       <c r="AA33" s="4">
         <f t="shared" ref="AA33" si="76">AA20/W20-1</f>
@@ -22298,7 +22293,7 @@
         <f t="shared" si="77"/>
         <v>1419.8679999999999</v>
       </c>
-      <c r="Y36" s="145">
+      <c r="Y36" s="11">
         <f t="shared" ref="Y36:AA36" si="78">Y37+Y42</f>
         <v>1489.8150000000001</v>
       </c>
@@ -22364,7 +22359,7 @@
       <c r="X37" s="10">
         <v>727.39400000000001</v>
       </c>
-      <c r="Y37" s="144">
+      <c r="Y37" s="10">
         <v>806.52800000000002</v>
       </c>
       <c r="Z37" s="15">
@@ -22425,7 +22420,7 @@
       <c r="X38" s="10">
         <v>89.835999999999999</v>
       </c>
-      <c r="Y38" s="144">
+      <c r="Y38" s="10">
         <v>97.542000000000002</v>
       </c>
       <c r="Z38" s="15">
@@ -22486,7 +22481,7 @@
       <c r="X39" s="10">
         <v>37.947000000000003</v>
       </c>
-      <c r="Y39" s="144">
+      <c r="Y39" s="10">
         <v>35.56</v>
       </c>
       <c r="Z39" s="15">
@@ -22547,7 +22542,7 @@
       <c r="X40" s="10">
         <v>98.117999999999995</v>
       </c>
-      <c r="Y40" s="144">
+      <c r="Y40" s="10">
         <v>91.852000000000004</v>
       </c>
       <c r="Z40" s="15">
@@ -22608,7 +22603,7 @@
       <c r="X41" s="10">
         <v>0</v>
       </c>
-      <c r="Y41" s="144">
+      <c r="Y41" s="10">
         <v>71.528999999999996</v>
       </c>
       <c r="Z41" s="15">
@@ -22669,7 +22664,7 @@
       <c r="X42" s="10">
         <v>692.47400000000005</v>
       </c>
-      <c r="Y42" s="144">
+      <c r="Y42" s="10">
         <v>683.28700000000003</v>
       </c>
       <c r="Z42" s="15">
@@ -22753,7 +22748,7 @@
         <f t="shared" si="84"/>
         <v>1645.7690000000002</v>
       </c>
-      <c r="Y43" s="145">
+      <c r="Y43" s="11">
         <f t="shared" ref="Y43:AA43" si="85">SUM(Y37:Y42)</f>
         <v>1786.2980000000002</v>
       </c>
@@ -22819,7 +22814,7 @@
       <c r="X44" s="10">
         <v>2202.739</v>
       </c>
-      <c r="Y44" s="144">
+      <c r="Y44" s="10">
         <v>2265.694</v>
       </c>
       <c r="Z44" s="15">
@@ -22880,7 +22875,7 @@
       <c r="X45" s="10">
         <v>776.81500000000005</v>
       </c>
-      <c r="Y45" s="144">
+      <c r="Y45" s="10">
         <v>972.64400000000001</v>
       </c>
       <c r="Z45" s="15">
@@ -22941,7 +22936,7 @@
       <c r="X46" s="10">
         <v>26.138000000000002</v>
       </c>
-      <c r="Y46" s="144">
+      <c r="Y46" s="10">
         <v>27.664000000000001</v>
       </c>
       <c r="Z46" s="15">
@@ -23002,7 +22997,7 @@
       <c r="X47" s="10">
         <v>3670.9830000000002</v>
       </c>
-      <c r="Y47" s="144">
+      <c r="Y47" s="10">
         <v>3770.9969999999998</v>
       </c>
       <c r="Z47" s="15">
@@ -23063,7 +23058,7 @@
       <c r="X48" s="10">
         <v>66.866</v>
       </c>
-      <c r="Y48" s="144">
+      <c r="Y48" s="10">
         <v>74.599000000000004</v>
       </c>
       <c r="Z48" s="15">
@@ -23124,7 +23119,7 @@
       <c r="X49" s="10">
         <v>21.939</v>
       </c>
-      <c r="Y49" s="144">
+      <c r="Y49" s="10">
         <v>21.939</v>
       </c>
       <c r="Z49" s="15">
@@ -23208,7 +23203,7 @@
         <f>SUM(X43:X49)</f>
         <v>8411.2489999999998</v>
       </c>
-      <c r="Y50" s="145">
+      <c r="Y50" s="11">
         <f t="shared" ref="Y50:AA50" si="90">SUM(Y43:Y49)</f>
         <v>8919.8350000000009</v>
       </c>
@@ -23274,7 +23269,7 @@
       <c r="X51" s="10">
         <v>196.86600000000001</v>
       </c>
-      <c r="Y51" s="144">
+      <c r="Y51" s="10">
         <v>203.48</v>
       </c>
       <c r="Z51" s="15">
@@ -23335,7 +23330,7 @@
       <c r="X52" s="10">
         <v>142.42500000000001</v>
       </c>
-      <c r="Y52" s="144">
+      <c r="Y52" s="10">
         <v>223.41</v>
       </c>
       <c r="Z52" s="15">
@@ -23396,7 +23391,7 @@
       <c r="X53" s="10">
         <v>171.61199999999999</v>
       </c>
-      <c r="Y53" s="144">
+      <c r="Y53" s="10">
         <v>169.631</v>
       </c>
       <c r="Z53" s="15">
@@ -23457,7 +23452,7 @@
       <c r="X54" s="10">
         <v>187.31700000000001</v>
       </c>
-      <c r="Y54" s="144">
+      <c r="Y54" s="10">
         <v>182.33099999999999</v>
       </c>
       <c r="Z54" s="15">
@@ -23518,7 +23513,7 @@
       <c r="X55" s="10">
         <v>254.14400000000001</v>
       </c>
-      <c r="Y55" s="144">
+      <c r="Y55" s="10">
         <v>264.30399999999997</v>
       </c>
       <c r="Z55" s="15">
@@ -23565,7 +23560,7 @@
       <c r="X56" s="10">
         <v>44.988999999999997</v>
       </c>
-      <c r="Y56" s="144"/>
+      <c r="Y56" s="10"/>
       <c r="Z56" s="15"/>
       <c r="AA56" s="10"/>
     </row>
@@ -23645,7 +23640,7 @@
         <f>SUM(X51:X56)</f>
         <v>997.35300000000007</v>
       </c>
-      <c r="Y57" s="145">
+      <c r="Y57" s="11">
         <f t="shared" ref="Y57:AA57" si="95">SUM(Y51:Y56)</f>
         <v>1043.1559999999999</v>
       </c>
@@ -23711,7 +23706,7 @@
       <c r="X58" s="10">
         <v>3903.3530000000001</v>
       </c>
-      <c r="Y58" s="144">
+      <c r="Y58" s="10">
         <v>4014.4540000000002</v>
       </c>
       <c r="Z58" s="15">
@@ -23772,7 +23767,7 @@
       <c r="X59" s="10">
         <v>84.228999999999999</v>
       </c>
-      <c r="Y59" s="144">
+      <c r="Y59" s="10">
         <v>83.298000000000002</v>
       </c>
       <c r="Z59" s="15">
@@ -23833,7 +23828,7 @@
       <c r="X60" s="10">
         <v>64.984999999999999</v>
       </c>
-      <c r="Y60" s="144">
+      <c r="Y60" s="10">
         <v>67.106999999999999</v>
       </c>
       <c r="Z60" s="15">
@@ -23917,7 +23912,7 @@
         <f>SUM(X57:X60)</f>
         <v>5049.92</v>
       </c>
-      <c r="Y61" s="145">
+      <c r="Y61" s="11">
         <f t="shared" ref="Y61:AA61" si="100">SUM(Y57:Y60)</f>
         <v>5208.0150000000003</v>
       </c>
@@ -23994,7 +23989,7 @@
         <f>X50-X61</f>
         <v>3361.3289999999997</v>
       </c>
-      <c r="Y62" s="144">
+      <c r="Y62" s="10">
         <f t="shared" ref="Y62:AA62" si="102">Y50-Y61</f>
         <v>3711.8200000000006</v>
       </c>
@@ -24013,17 +24008,14 @@
       <c r="E64" s="50"/>
       <c r="F64" s="50"/>
       <c r="G64" s="51"/>
-      <c r="Y64" s="149"/>
       <c r="Z64" s="16"/>
     </row>
     <row r="82" spans="7:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G82" s="41"/>
-      <c r="Y82" s="150"/>
       <c r="Z82" s="41"/>
     </row>
     <row r="83" spans="7:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G83" s="16"/>
-      <c r="Y83" s="149"/>
       <c r="Z83" s="16"/>
     </row>
   </sheetData>
@@ -36257,14 +36249,14 @@
       <c r="D1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="133" t="s">
+      <c r="H1" s="134" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
-      <c r="L1" s="134"/>
-      <c r="M1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="136"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12">
@@ -36767,10 +36759,10 @@
         <f t="shared" si="0"/>
         <v>2.6708175927015354E-2</v>
       </c>
-      <c r="H17" s="136" t="s">
+      <c r="H17" s="137" t="s">
         <v>131</v>
       </c>
-      <c r="I17" s="137"/>
+      <c r="I17" s="138"/>
       <c r="M17" s="79"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -36784,8 +36776,8 @@
         <f t="shared" si="0"/>
         <v>-3.2427289180687158E-2</v>
       </c>
-      <c r="H18" s="138"/>
-      <c r="I18" s="139"/>
+      <c r="H18" s="139"/>
+      <c r="I18" s="140"/>
       <c r="M18" s="79"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -37358,14 +37350,14 @@
         <f t="shared" si="0"/>
         <v>-1.0339540305585704E-2</v>
       </c>
-      <c r="H43" s="140" t="s">
+      <c r="H43" s="141" t="s">
         <v>125</v>
       </c>
-      <c r="I43" s="141"/>
-      <c r="J43" s="141"/>
-      <c r="K43" s="141"/>
-      <c r="L43" s="141"/>
-      <c r="M43" s="142"/>
+      <c r="I43" s="142"/>
+      <c r="J43" s="142"/>
+      <c r="K43" s="142"/>
+      <c r="L43" s="142"/>
+      <c r="M43" s="143"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="12">

</xml_diff>